<commit_message>
separate MessageBased and SDK connections
</commit_message>
<xml_diff>
--- a/msl/examples/equipment/example-equipment-connections-database.xlsx
+++ b/msl/examples/equipment/example-equipment-connections-database.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\git\msl-equipment\msl\examples\equipment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.borbely\code\git\msl-equipment\msl\examples\equipment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7560" yWindow="0" windowWidth="18255" windowHeight="11955"/>
+    <workbookView xWindow="8505" yWindow="0" windowWidth="18255" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Equipment" sheetId="1" r:id="rId1"/>
@@ -280,9 +280,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Communicating to this equipment is done through a DLL library provided by the manufacturer.
+          <t>Communicating to this equipment is done through a the SDK provided by the manufacturer.
 The following structure is used:
-LIB::PythonClassName::PathToLibraryFile</t>
+SDK::PythonWrapperClassName::PathToLibraryFile</t>
         </r>
       </text>
     </comment>
@@ -793,9 +793,6 @@
     <t>SR850 DSP</t>
   </si>
   <si>
-    <t>LIB::Bentham::C:\goni\lib\bentham.dll</t>
-  </si>
-  <si>
     <t>GPIB1::8</t>
   </si>
   <si>
@@ -845,6 +842,9 @@
   </si>
   <si>
     <t>G10014</t>
+  </si>
+  <si>
+    <t>SDK::Bentham::C:\goni\lib\bentham.dll</t>
   </si>
 </sst>
 </file>
@@ -1322,21 +1322,21 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="35.59765625" customWidth="1"/>
-    <col min="3" max="3" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.59765625" customWidth="1"/>
-    <col min="6" max="6" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.3984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="171.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1454,7 +1454,7 @@
       </c>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -1564,7 +1564,7 @@
       </c>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1674,7 +1674,7 @@
       </c>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1700,7 +1700,7 @@
       </c>
       <c r="J13" s="11"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="J14" s="11"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1752,7 +1752,7 @@
       </c>
       <c r="J15" s="11"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
@@ -1778,7 +1778,7 @@
       </c>
       <c r="J16" s="11"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="J18" s="11"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="J19" s="11"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1882,7 +1882,7 @@
       </c>
       <c r="J20" s="11"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="J21" s="11"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
@@ -1968,7 +1968,7 @@
       </c>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>7</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
@@ -2065,20 +2065,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.3984375" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.86328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.86328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.1328125" style="16"/>
-    <col min="9" max="9" width="43.3984375" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="16"/>
+    <col min="6" max="6" width="46.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="16"/>
+    <col min="9" max="9" width="43.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>102</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>4</v>
       </c>
@@ -2106,17 +2106,17 @@
         <v>104</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>110</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>106</v>
       </c>
@@ -2124,19 +2124,19 @@
         <v>105</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>110</v>
       </c>
       <c r="E3" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>4</v>
       </c>
@@ -2150,11 +2150,11 @@
         <v>110</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>108</v>
       </c>
@@ -2162,17 +2162,17 @@
         <v>107</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>109</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>111</v>
       </c>
@@ -2180,17 +2180,17 @@
         <v>112</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>110</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>4</v>
       </c>
@@ -2204,11 +2204,11 @@
         <v>109</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>17</v>
       </c>
@@ -2216,19 +2216,19 @@
         <v>113</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>110</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>114</v>
       </c>
@@ -2236,19 +2236,19 @@
         <v>115</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>109</v>
       </c>
       <c r="E9" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>4</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>110</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10"/>

</xml_diff>